<commit_message>
Fixed bi-linear interpolation for vol surface.
</commit_message>
<xml_diff>
--- a/gbm/vol-surface-data-2022-06-30.xlsx
+++ b/gbm/vol-surface-data-2022-06-30.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitLab\stochastic_process_calibration_2022\gbm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2452661F-F25D-45B5-A618-03C880EF6C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0166C2CD-E3B2-43E6-BC05-A119E6401868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="1" xr2:uid="{A8F70B9E-AEBD-4856-A6E0-756ECC06B53E}"/>
   </bookViews>
@@ -3272,7 +3272,7 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>